<commit_message>
i trying to make update
</commit_message>
<xml_diff>
--- a/tripleCRUD/triple_site/sheet/triple_sheet.xlsx
+++ b/tripleCRUD/triple_site/sheet/triple_sheet.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -505,6 +505,23 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>peiper</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>is</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>party member</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
1/2 of the week02 task
</commit_message>
<xml_diff>
--- a/tripleCRUD/triple_site/sheet/triple_sheet.xlsx
+++ b/tripleCRUD/triple_site/sheet/triple_sheet.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -440,102 +440,136 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>peiper</t>
+          <t>peiper:Person</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">is </t>
+          <t>born</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>officer</t>
+          <t>30 January 1915</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>peiper</t>
+          <t>peiper:Person</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>born</t>
+          <t>is_a</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>30 January 1915</t>
+          <t>soldier</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>peiper</t>
+          <t>peiper:Person</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>is</t>
+          <t>die</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>soldier</t>
+          <t>14 July 1976</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>peiper</t>
+          <t>peiper:Person</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>die</t>
+          <t>is_a</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>14 July 1976</t>
+          <t>nazi member</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>peiper</t>
+          <t>peiper:Person</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>is</t>
+          <t>is_a</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>nazi member</t>
+          <t>German</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>peiper:Person</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>is_a</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>officer</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>peiper:Person</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>born_in</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Wilmersdorf, Berlin, Germany</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>himler:Person</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>know</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>peiper</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>is</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>German</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
1/2 of the week task (UI update)
</commit_message>
<xml_diff>
--- a/tripleCRUD/triple_site/sheet/triple_sheet.xlsx
+++ b/tripleCRUD/triple_site/sheet/triple_sheet.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -445,12 +445,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>born</t>
+          <t>is_a</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>30 January 1915</t>
+          <t>soldier</t>
         </is>
       </c>
     </row>
@@ -462,12 +462,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>is_a</t>
+          <t>die</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>soldier</t>
+          <t>14 July 1976</t>
         </is>
       </c>
     </row>
@@ -479,12 +479,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>die</t>
+          <t>is_a</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>14 July 1976</t>
+          <t>nazi member</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>nazi member</t>
+          <t>German</t>
         </is>
       </c>
     </row>
@@ -518,7 +518,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>German</t>
+          <t>officer</t>
         </is>
       </c>
     </row>
@@ -530,29 +530,29 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>is_a</t>
+          <t>born_in</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>officer</t>
+          <t>Wilmersdorf, Berlin, Germany</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>peiper:Person</t>
+          <t>himler:Person</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>born_in</t>
+          <t>know</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Wilmersdorf, Berlin, Germany</t>
+          <t>peiper</t>
         </is>
       </c>
     </row>
@@ -564,12 +564,29 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>know</t>
+          <t>born</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>peiper</t>
+          <t>7 October 1900</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>himler:Person</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>die</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>23 May 1945</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
2/2 of Week02 task complete
</commit_message>
<xml_diff>
--- a/tripleCRUD/triple_site/sheet/triple_sheet.xlsx
+++ b/tripleCRUD/triple_site/sheet/triple_sheet.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -445,63 +445,63 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>is_a</t>
+          <t>born_in</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>soldier</t>
+          <t>Wilmersdorf, Berlin, Germany</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>peiper:Person</t>
+          <t>himler:Person</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>die</t>
+          <t>know</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>14 July 1976</t>
+          <t>peiper</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>peiper:Person</t>
+          <t>himler:Person</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>is_a</t>
+          <t>born</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>nazi member</t>
+          <t>7 October 1900</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>peiper:Person</t>
+          <t>himler:Person</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>is_a</t>
+          <t>die</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>German</t>
+          <t>23 May 1945</t>
         </is>
       </c>
     </row>
@@ -518,7 +518,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>officer</t>
+          <t>soldier</t>
         </is>
       </c>
     </row>
@@ -530,63 +530,131 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>born_in</t>
+          <t>is_a</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Wilmersdorf, Berlin, Germany</t>
+          <t>nazi member</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>himler:Person</t>
+          <t>peiper:Person</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>know</t>
+          <t>born</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>peiper</t>
+          <t>30 January 1915</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>himler:Person</t>
+          <t>peiper:Person</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>born</t>
+          <t>is_a</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>7 October 1900</t>
+          <t>German</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>peiper:Person</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>die</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>14 July 1976</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>himler:Person</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>die</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>23 May 1945</t>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>is_a</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>officer</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>himler:Person</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>is_a</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>commander</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>peiper:Person</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>is_a</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>commander</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>peiper:Person</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>is_a</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>officer</t>
         </is>
       </c>
     </row>

</xml_diff>